<commit_message>
Mise à jour des corrections d'affichage frontend et du backend, avec nettoyage des fichiers ignorés
</commit_message>
<xml_diff>
--- a/backend/reports/resultats_scoring_test_clients_100_conso.xlsx
+++ b/backend/reports/resultats_scoring_test_clients_100_conso.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,20 +486,30 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>client_identifier</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>scoring_PC</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>scoring_PI</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>score_appetence</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>client_identifier</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>observations_forces</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>observations_faiblesses</t>
         </is>
@@ -537,21 +547,25 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Client 1</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Age Faible (24)</t>
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -587,21 +601,25 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Client 2</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Age Faible (37)</t>
+        <v>2</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -637,21 +655,25 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Client 3</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (49)</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>3</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (41.00%)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -687,21 +709,25 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Client 4</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Age Élevé (63)</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>4</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -737,21 +763,25 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Client 5</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Age Élevé (48)</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -787,21 +817,25 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Client 6</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (0); Age Faible (39)</t>
+        <v>6</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -837,21 +871,25 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Client 7</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Age Faible (22)</t>
+        <v>7</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -887,21 +925,25 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Client 8</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Age Élevé (48)</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>8</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (37.00%)</t>
         </is>
       </c>
     </row>
@@ -937,21 +979,25 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Client 9</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Age Faible (32)</t>
+        <v>9</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -987,21 +1033,25 @@
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Client 10</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (61)</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>10</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -1037,21 +1087,25 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Client 11</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (34)</t>
+        <v>11</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -1087,21 +1141,25 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Client 12</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Age Élevé (54)</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>12</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -1137,21 +1195,25 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Client 13</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Age Faible (36)</t>
+        <v>13</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (37.00%)</t>
         </is>
       </c>
     </row>
@@ -1187,21 +1249,25 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Client 14</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (27)</t>
+        <v>14</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -1237,21 +1303,25 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Client 15</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>Age Élevé (61)</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>15</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -1287,21 +1357,25 @@
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Client 16</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (51)</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>16</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -1337,21 +1411,25 @@
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Client 17</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Age Élevé (66)</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>17</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -1387,21 +1465,25 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Client 18</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (42)</t>
+        <v>18</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -1437,21 +1519,25 @@
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Client 19</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (54)</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>19</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (33.00%)</t>
         </is>
       </c>
     </row>
@@ -1487,21 +1573,25 @@
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Client 20</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (45)</t>
+        <v>20</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (41.00%)</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -1537,21 +1627,25 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Client 21</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>Age Faible (32)</t>
+        <v>21</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -1587,21 +1681,25 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Client 22</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>Age Faible (37)</t>
+        <v>22</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (33.00%)</t>
         </is>
       </c>
     </row>
@@ -1637,21 +1735,25 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Client 23</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>Age Faible (30)</t>
+        <v>23</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -1687,21 +1789,25 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Client 24</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (37)</t>
+        <v>24</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -1737,21 +1843,25 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Client 25</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (60)</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>25</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -1787,21 +1897,25 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Client 26</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>Age Élevé (48)</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>26</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -1837,21 +1951,25 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Client 27</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (35)</t>
+        <v>27</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (30.00%)</t>
         </is>
       </c>
     </row>
@@ -1887,21 +2005,25 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Client 28</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (58)</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>28</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -1937,21 +2059,25 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Client 29</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Age Élevé (65)</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>29</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -1987,21 +2113,25 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Client 30</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (45)</t>
+        <v>30</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2037,21 +2167,25 @@
         <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Client 31</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (64)</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>31</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -2087,21 +2221,25 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Client 32</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>Age Faible (21)</t>
+        <v>32</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -2137,21 +2275,25 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>Client 33</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (41)</t>
+        <v>33</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2187,21 +2329,25 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>Client 34</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (61)</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>34</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -2237,21 +2383,25 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>Client 35</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>Age Élevé (62)</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>35</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -2287,21 +2437,25 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>Client 36</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>Age Faible (26)</t>
+        <v>36</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -2337,21 +2491,25 @@
         <v>1</v>
       </c>
       <c r="K38" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Client 37</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (64)</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>37</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -2387,21 +2545,25 @@
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>Client 38</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (67)</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>38</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -2437,21 +2599,25 @@
         <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>Client 39</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>Age Élevé (69)</t>
-        </is>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>39</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (33.00%)</t>
         </is>
       </c>
     </row>
@@ -2487,21 +2653,25 @@
         <v>1</v>
       </c>
       <c r="K41" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>Client 40</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (49)</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>40</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2537,21 +2707,25 @@
         <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>Client 41</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (49)</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>41</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2587,21 +2761,25 @@
         <v>1</v>
       </c>
       <c r="K43" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>Client 42</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (56)</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>42</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (41.00%)</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2637,21 +2815,25 @@
         <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>Client 43</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (38)</t>
+        <v>43</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2687,21 +2869,25 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>Client 44</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (61)</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>44</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -2737,21 +2923,25 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Client 45</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (59)</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>45</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -2787,21 +2977,25 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Client 46</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (56)</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>46</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -2837,21 +3031,25 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Client 47</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Age Élevé (63)</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>47</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -2887,21 +3085,25 @@
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>Client 48</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (44)</t>
+        <v>48</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -2937,21 +3139,25 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Client 49</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Age Élevé (64)</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>49</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -2987,21 +3193,25 @@
         <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Client 50</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (53)</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>50</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3037,21 +3247,25 @@
         <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>Client 51</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>Age Faible (25)</t>
+        <v>51</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -3087,21 +3301,25 @@
         <v>1</v>
       </c>
       <c r="K53" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Client 52</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (0); Age Faible (36)</t>
+        <v>52</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -3137,21 +3355,25 @@
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>Client 53</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>Age Élevé (46)</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (0)</t>
+        <v>53</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3187,21 +3409,25 @@
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>Client 54</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>Age Faible (36)</t>
+        <v>54</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -3237,21 +3463,25 @@
         <v>1</v>
       </c>
       <c r="K56" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>Client 55</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>Age Faible (22)</t>
+        <v>55</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -3287,21 +3517,25 @@
         <v>0</v>
       </c>
       <c r="K57" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>Client 56</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (0); Age Faible (39)</t>
+        <v>56</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3337,21 +3571,25 @@
         <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>Client 57</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (52)</t>
-        </is>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>57</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3387,21 +3625,25 @@
         <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>Client 58</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>Age Faible (27)</t>
+        <v>58</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -3437,21 +3679,25 @@
         <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>Client 59</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>Age Faible (32)</t>
+        <v>59</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (31.00%)</t>
         </is>
       </c>
     </row>
@@ -3487,21 +3733,25 @@
         <v>1</v>
       </c>
       <c r="K61" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Client 60</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>Age Faible (19)</t>
+        <v>60</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (31.00%)</t>
         </is>
       </c>
     </row>
@@ -3537,21 +3787,25 @@
         <v>1</v>
       </c>
       <c r="K62" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>Client 61</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (59)</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>61</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -3587,21 +3841,25 @@
         <v>0</v>
       </c>
       <c r="K63" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>Client 62</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>Age Faible (39)</t>
+        <v>62</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3637,21 +3895,25 @@
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>Client 63</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (65)</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>63</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -3687,21 +3949,25 @@
         <v>1</v>
       </c>
       <c r="K65" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>Client 64</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (52)</t>
-        </is>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>64</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3737,21 +4003,25 @@
         <v>0</v>
       </c>
       <c r="K66" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>Client 65</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (56)</t>
-        </is>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>65</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -3787,21 +4057,25 @@
         <v>1</v>
       </c>
       <c r="K67" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>Client 66</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>Age Faible (36)</t>
+        <v>66</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -3837,21 +4111,25 @@
         <v>0</v>
       </c>
       <c r="K68" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>Client 67</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (64)</t>
-        </is>
-      </c>
-      <c r="N68" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>67</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (37.00%)</t>
         </is>
       </c>
     </row>
@@ -3887,21 +4165,25 @@
         <v>0</v>
       </c>
       <c r="K69" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Client 68</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (29)</t>
+        <v>68</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (30.00%)</t>
         </is>
       </c>
     </row>
@@ -3937,21 +4219,25 @@
         <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Client 69</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>Age Élevé (51)</t>
-        </is>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>69</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -3987,21 +4273,25 @@
         <v>1</v>
       </c>
       <c r="K71" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>Client 70</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>Age Élevé (62)</t>
-        </is>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>70</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (37.00%)</t>
         </is>
       </c>
     </row>
@@ -4037,21 +4327,25 @@
         <v>1</v>
       </c>
       <c r="K72" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>Client 71</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (0); Age Faible (37)</t>
+        <v>71</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -4087,21 +4381,25 @@
         <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>Client 72</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>Age Élevé (68)</t>
-        </is>
-      </c>
-      <c r="N73" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (0)</t>
+        <v>72</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (30.00%)</t>
         </is>
       </c>
     </row>
@@ -4137,21 +4435,25 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Client 73</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>Age Faible (24)</t>
+        <v>73</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -4187,21 +4489,25 @@
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>Client 74</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N75" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (41)</t>
+        <v>74</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (41.00%)</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -4237,21 +4543,25 @@
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>Client 75</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (20)</t>
+        <v>75</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (34.00%)</t>
         </is>
       </c>
     </row>
@@ -4287,21 +4597,25 @@
         <v>1</v>
       </c>
       <c r="K77" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>Client 76</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (23)</t>
+        <v>76</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -4337,21 +4651,25 @@
         <v>1</v>
       </c>
       <c r="K78" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>Client 77</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (50)</t>
-        </is>
-      </c>
-      <c r="N78" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>77</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -4387,21 +4705,25 @@
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>Client 78</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (51)</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>78</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (41.00%)</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -4437,21 +4759,25 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Client 79</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (50)</t>
-        </is>
-      </c>
-      <c r="N80" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>79</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -4487,21 +4813,25 @@
         <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Client 80</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>Age Élevé (46)</t>
-        </is>
-      </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>80</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M81" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (38.00%)</t>
         </is>
       </c>
     </row>
@@ -4537,21 +4867,25 @@
         <v>0</v>
       </c>
       <c r="K82" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Client 81</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>Age Faible (40)</t>
+        <v>81</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M82" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (40.00%)</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -4587,21 +4921,25 @@
         <v>0</v>
       </c>
       <c r="K83" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Client 82</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N83" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (21)</t>
+        <v>82</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M83" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -4637,21 +4975,25 @@
         <v>1</v>
       </c>
       <c r="K84" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Client 83</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>Age Faible (22)</t>
+        <v>83</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M84" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -4687,21 +5029,25 @@
         <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Client 84</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>Age Élevé (51)</t>
-        </is>
-      </c>
-      <c r="N85" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>84</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -4737,21 +5083,25 @@
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>Client 85</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N86" t="inlineStr">
-        <is>
-          <t>Age Faible (33)</t>
+        <v>85</v>
+      </c>
+      <c r="L86" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M86" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (39.00%)</t>
         </is>
       </c>
     </row>
@@ -4787,21 +5137,25 @@
         <v>1</v>
       </c>
       <c r="K87" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Client 86</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>Age Élevé (57)</t>
-        </is>
-      </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>86</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (43.00%)</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -4837,21 +5191,25 @@
         <v>1</v>
       </c>
       <c r="K88" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>Client 87</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (64)</t>
-        </is>
-      </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>87</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M88" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -4887,21 +5245,25 @@
         <v>1</v>
       </c>
       <c r="K89" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Client 88</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>Age Élevé (60)</t>
-        </is>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>88</v>
+      </c>
+      <c r="L89" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M89" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N89" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -4937,21 +5299,25 @@
         <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>Client 89</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (59)</t>
-        </is>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>89</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M90" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N90" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -4987,21 +5353,25 @@
         <v>1</v>
       </c>
       <c r="K91" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>Client 90</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (20)</t>
+        <v>90</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M91" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N91" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -5037,21 +5407,25 @@
         <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>Client 91</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>Age Élevé (60)</t>
-        </is>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>91</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M92" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>
@@ -5087,21 +5461,25 @@
         <v>0</v>
       </c>
       <c r="K93" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>Client 92</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (66)</t>
-        </is>
-      </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>92</v>
+      </c>
+      <c r="L93" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M93" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N93" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (30.00%)</t>
         </is>
       </c>
     </row>
@@ -5137,21 +5515,25 @@
         <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>Client 93</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>Age Élevé (59)</t>
-        </is>
-      </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>93</v>
+      </c>
+      <c r="L94" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M94" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N94" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (37.00%)</t>
         </is>
       </c>
     </row>
@@ -5187,21 +5569,25 @@
         <v>1</v>
       </c>
       <c r="K95" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>Client 94</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0); Age Élevé (66)</t>
-        </is>
-      </c>
-      <c r="N95" t="inlineStr">
-        <is>
-          <t>N/A</t>
+        <v>94</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M95" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N95" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (32.00%)</t>
         </is>
       </c>
     </row>
@@ -5237,21 +5623,25 @@
         <v>0</v>
       </c>
       <c r="K96" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>Client 95</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>Taux endettement Faible (0)</t>
-        </is>
-      </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>Age Faible (31)</t>
+        <v>95</v>
+      </c>
+      <c r="L96" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M96" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="N96" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -5287,21 +5677,25 @@
         <v>0</v>
       </c>
       <c r="K97" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>Client 96</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>Age Élevé (50)</t>
-        </is>
-      </c>
-      <c r="N97" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>96</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M97" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (42.00%)</t>
+        </is>
+      </c>
+      <c r="P97" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -5337,21 +5731,25 @@
         <v>1</v>
       </c>
       <c r="K98" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>Client 97</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N98" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (45)</t>
+        <v>97</v>
+      </c>
+      <c r="L98" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M98" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N98" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>Score d'appétence modéré (41.00%)</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>Aucune faiblesse majeure spécifique identifiée.</t>
         </is>
       </c>
     </row>
@@ -5387,21 +5785,25 @@
         <v>0</v>
       </c>
       <c r="K99" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>Client 98</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>Age Élevé (58)</t>
-        </is>
-      </c>
-      <c r="N99" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1)</t>
+        <v>98</v>
+      </c>
+      <c r="L99" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M99" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N99" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (37.00%)</t>
         </is>
       </c>
     </row>
@@ -5437,21 +5839,25 @@
         <v>1</v>
       </c>
       <c r="K100" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>Client 99</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N100" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (32)</t>
+        <v>99</v>
+      </c>
+      <c r="L100" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M100" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N100" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (36.00%)</t>
         </is>
       </c>
     </row>
@@ -5487,21 +5893,25 @@
         <v>1</v>
       </c>
       <c r="K101" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>Client 100</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N101" t="inlineStr">
-        <is>
-          <t>Taux endettement Élevé (1); Age Faible (21)</t>
+        <v>100</v>
+      </c>
+      <c r="L101" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M101" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N101" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>Aucune force majeure spécifique identifiée.</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>Score d'appétence globalement faible (35.00%)</t>
         </is>
       </c>
     </row>

</xml_diff>